<commit_message>
Voorbeeld xlsx werkt naar behoren
</commit_message>
<xml_diff>
--- a/portfolio_voorbeeld.xlsx
+++ b/portfolio_voorbeeld.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="instellingen" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="46">
   <si>
     <t xml:space="preserve">variabelen</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t xml:space="preserve">ilo5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indicator 5a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indicator5b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indicator5c</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="1" sqref="C14 G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -387,8 +396,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1229,7 +1238,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="1" sqref="C14 C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2093,8 +2102,8 @@
   </sheetPr>
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2309,7 +2318,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -2324,15 +2333,23 @@
         <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4"/>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>

</xml_diff>